<commit_message>
Adding custom annotation to Framework
</commit_message>
<xml_diff>
--- a/src/test/resources/data/testData.xlsx
+++ b/src/test/resources/data/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\SeleniumFramework\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756D528A-D86C-4233-BFD4-AF8105485DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD489E8E-6946-4542-AC96-FDDACC4C5A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E0C4D6F5-A401-4477-BC0E-59177A2A72AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E0C4D6F5-A401-4477-BC0E-59177A2A72AB}"/>
   </bookViews>
   <sheets>
     <sheet name="AllTests" sheetId="1" r:id="rId1"/>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DD5885-04C1-4DBC-9785-DCEC90AEF89B}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -531,7 +531,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>25</v>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F0D0E4-DB25-41AE-8BD5-B986C9C1C8D7}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -699,7 +699,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>

</xml_diff>